<commit_message>
finished preliminary circuit and started BOM
</commit_message>
<xml_diff>
--- a/EE333-BOM.xlsx
+++ b/EE333-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\OneDrive\Documents\EE333-Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfro\OneDrive\Documents\EE333-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8AFC0E-EEEB-4E4C-9593-D1DAE3E8FFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F965DF6E-7C0E-4BA7-A519-9D3503810F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6435" windowWidth="16440" windowHeight="28440" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Op Amp</t>
   </si>
@@ -65,35 +64,47 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/rochester-electronics-llc/LT1815CS6-TRMPBF/15644489</t>
-  </si>
-  <si>
-    <t>Regulator</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/texas-instruments/NE555P/277057</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LT1576CS8-PBF/889050</t>
-  </si>
-  <si>
-    <t>r1</t>
-  </si>
-  <si>
-    <t>r2</t>
-  </si>
-  <si>
-    <t>vout</t>
-  </si>
-  <si>
-    <t>need to select the correct inductor</t>
+    <t>https://www.digikey.com/en/products/detail/hammond-manufacturing/166LA12/2182731</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LMC660CN-NOPB/32519</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/smc-diode-solutions/SF26G/6022671</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>other capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cornell-dubilier-illinois-capacitor/109LBB016M2BC/5410933</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cornell-dubilier-illinois-capacitor/105CKH050M/5410526</t>
+  </si>
+  <si>
+    <t>one last capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/URZ2AR22MDD1TD/4320687</t>
+  </si>
+  <si>
+    <t>resistors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +116,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,14 +146,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E675021-61AE-4F38-A35F-D09CECFBF373}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +482,7 @@
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -476,72 +499,138 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.06</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <f>(C4)*4</f>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>17.72</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>17.72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="K11">
-        <f>K12*(K13-1.21)/1.21</f>
-        <v>19793.388429752067</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J12" t="s">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.47</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <f>C6*2</f>
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="K12">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J14" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{25FE2449-C20D-40B9-8937-BDCD6E6C3FEB}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{908829E4-CB96-4877-9E3D-32EB117B23E5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="136" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="136" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added bom desctriptions for missing components :)
</commit_message>
<xml_diff>
--- a/EE333-BOM.xlsx
+++ b/EE333-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfro\OneDrive\Documents\EE333-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F965DF6E-7C0E-4BA7-A519-9D3503810F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACACF98-DCF9-4163-B309-480FA6DAC1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Op Amp</t>
   </si>
@@ -95,6 +95,42 @@
   </si>
   <si>
     <t>resistors</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>250k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>2.5k</t>
+  </si>
+  <si>
+    <t>pots</t>
+  </si>
+  <si>
+    <t>1k to 0</t>
+  </si>
+  <si>
+    <t>some wide range around 100k, idk</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>preferably connects all three voltages or disconnects the 120V wall power</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>PNP</t>
   </si>
 </sst>
 </file>
@@ -470,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E675021-61AE-4F38-A35F-D09CECFBF373}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +518,7 @@
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -499,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -516,7 +552,7 @@
         <v>6.12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -533,7 +569,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -551,7 +587,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -568,7 +604,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -586,7 +622,7 @@
         <v>6.94</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -603,7 +639,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -620,9 +656,84 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished abstract, work needs to be done on part specifics
</commit_message>
<xml_diff>
--- a/EE333-BOM.xlsx
+++ b/EE333-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfro\OneDrive\Documents\EE333-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACACF98-DCF9-4163-B309-480FA6DAC1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6EF96-94A7-4EE4-8A64-F3977AB2536D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
+    <workbookView xWindow="-4836" yWindow="4632" windowWidth="14820" windowHeight="10044" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Op Amp</t>
   </si>
@@ -94,43 +94,88 @@
     <t>https://www.digikey.com/en/products/detail/nichicon/URZ2AR22MDD1TD/4320687</t>
   </si>
   <si>
-    <t>resistors</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>250k</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>2.5k</t>
-  </si>
-  <si>
     <t>pots</t>
   </si>
   <si>
-    <t>1k to 0</t>
-  </si>
-  <si>
-    <t>some wide range around 100k, idk</t>
-  </si>
-  <si>
     <t>switch</t>
   </si>
   <si>
-    <t>preferably connects all three voltages or disconnects the 120V wall power</t>
-  </si>
-  <si>
     <t>NPN</t>
   </si>
   <si>
     <t>PNP</t>
+  </si>
+  <si>
+    <t>In kit?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CFR-25JT-52-1M/9098565</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CFR50SJT-52-1K/9099728</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1k resistor</t>
+  </si>
+  <si>
+    <t>1M resistor</t>
+  </si>
+  <si>
+    <t>100k resistor</t>
+  </si>
+  <si>
+    <t>10k resistor</t>
+  </si>
+  <si>
+    <t>5k resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CFR-12JT-52-10K/9098021</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CFR25SJT-52-100K/9098845</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/PTN10-B200SB20/16628511</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/PTN10-E01SB20/16628490</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nidec-copal-electronics/ET310A12-Z/5086810</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/BUL138/1037756</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/D45H8G/918452</t>
+  </si>
+  <si>
+    <t>total cost:</t>
+  </si>
+  <si>
+    <t>8 pin conn</t>
+  </si>
+  <si>
+    <t>16 pin conn</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adam-tech/ICS-308-T/9829299</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adam-tech/ICM-316-1-GT-HT/9833008</t>
   </si>
 </sst>
 </file>
@@ -506,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E675021-61AE-4F38-A35F-D09CECFBF373}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,6 +579,9 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -551,6 +599,9 @@
       <c r="E2" s="2">
         <v>6.12</v>
       </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -567,6 +618,9 @@
       </c>
       <c r="E3" s="2">
         <v>0.48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -586,6 +640,9 @@
         <f>(C4)*4</f>
         <v>1.52</v>
       </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -603,6 +660,9 @@
       <c r="E5" s="2">
         <v>17.72</v>
       </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -621,6 +681,9 @@
         <f>C6*2</f>
         <v>6.94</v>
       </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -638,6 +701,9 @@
       <c r="E7" s="2">
         <v>0.27</v>
       </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -655,45 +721,105 @@
       <c r="E8" s="2">
         <v>0.33</v>
       </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.11</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
+      <c r="E9" s="2">
+        <v>0.77</v>
+      </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.1</v>
+      </c>
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.1</v>
+      </c>
       <c r="D11">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.4</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.1</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -701,39 +827,149 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.65</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
+      <c r="E14" s="2">
+        <f>C14*2</f>
+        <v>1.3</v>
+      </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.65</v>
+      </c>
       <c r="D15">
         <v>2</v>
       </c>
+      <c r="E15" s="2">
+        <v>1.3</v>
+      </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2">
+        <v>10.3</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10.3</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.59</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="2">
+        <f>SUM(E2:E20)</f>
+        <v>51.149999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
began kicad design, tried to convert any components we had to being available in the lab kit. More work definitely needs to be done to ensure that we have the right footprints, and a proper bom put together.
</commit_message>
<xml_diff>
--- a/EE333-BOM.xlsx
+++ b/EE333-BOM.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfro\OneDrive\Documents\EE333-Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\OneDrive\Documents\EE333-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6EF96-94A7-4EE4-8A64-F3977AB2536D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2169D1-865E-4E9E-AD9E-C3DB19BE59A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4836" yWindow="4632" windowWidth="14820" windowHeight="10044" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
+    <workbookView xWindow="28680" yWindow="-6435" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{7106F7B5-535B-4303-8754-DB76A419050D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="KiCad Redesign" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Op Amp</t>
   </si>
@@ -553,17 +554,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E675021-61AE-4F38-A35F-D09CECFBF373}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -583,7 +585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -603,7 +605,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -623,7 +625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -644,7 +646,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -664,7 +666,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -685,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -705,7 +707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -725,7 +727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -745,7 +747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -765,7 +767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -785,7 +787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -805,7 +807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -825,7 +827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -846,7 +848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -863,7 +865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -883,7 +885,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -903,7 +905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -923,7 +925,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -943,7 +945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -963,7 +965,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>42</v>
       </c>
@@ -980,4 +982,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="136" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E95EAAE-9DEC-44BB-A393-B7DA9A580DE2}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>